<commit_message>
Factorized the data legend to a separate text file
</commit_message>
<xml_diff>
--- a/jss13_ht20.xlsx
+++ b/jss13_ht20.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsyuch\Desktop\Utbildningar\Masterutbildning\Data science\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\redho\Documents\gits\labAssignmentsForStatisticalMethods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E109CC27-3605-4579-8FE3-A9E4154F9702}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD18A50-15AA-419B-9C08-02C1B02FA1BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{039FF9D7-ACF4-48DA-B635-5B4DE3137A46}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="38700" windowHeight="15435" xr2:uid="{039FF9D7-ACF4-48DA-B635-5B4DE3137A46}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Id</t>
   </si>
@@ -70,24 +70,6 @@
   </si>
   <si>
     <t>income</t>
-  </si>
-  <si>
-    <t>gender ( male =1, female =2)</t>
-  </si>
-  <si>
-    <t>attend = attendance at meeting (yes = 1, no = 2)</t>
-  </si>
-  <si>
-    <t>skill = rated skill (unskilled = 1, semi-skilled = 2, fairly skilled = 3, highly skilled = 4)</t>
-  </si>
-  <si>
-    <t>prody = rated productivity (very poor = 1, poor = 2, average = 3, good = 4, very good = 5)</t>
-  </si>
-  <si>
-    <t>qual = rated quality (very poor = 1, poor = 2, average = 3, good= 4, very good = 5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ethnicgp = ethnic group  (1 = White, 2 = Asian, 3 = West Indian, 4 = African, 5 = other) </t>
   </si>
 </sst>
 </file>
@@ -442,13 +424,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE3C3EA-22F1-48A8-870F-DC8C6537F1CD}">
   <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -495,7 +477,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -536,7 +518,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -580,7 +562,7 @@
         <v>14.6</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -627,7 +609,7 @@
         <v>17.8</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -674,7 +656,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -721,7 +703,7 @@
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -768,7 +750,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -812,7 +794,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -859,7 +841,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -906,7 +888,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -953,7 +935,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1000,7 +982,7 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1044,7 +1026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1091,7 +1073,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1138,7 +1120,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1185,7 +1167,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1232,7 +1214,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1279,7 +1261,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1326,7 +1308,7 @@
         <v>13.4</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1373,7 +1355,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1420,7 +1402,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1464,7 +1446,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1511,7 +1493,7 @@
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1558,7 +1540,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1605,7 +1587,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1652,7 +1634,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1699,7 +1681,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1746,7 +1728,7 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1793,7 +1775,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1840,7 +1822,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1887,7 +1869,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1931,7 +1913,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1978,7 +1960,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2025,7 +2007,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2072,7 +2054,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2119,7 +2101,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2166,7 +2148,7 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2213,7 +2195,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2260,7 +2242,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2307,7 +2289,7 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2354,7 +2336,7 @@
         <v>13.4</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2401,7 +2383,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2448,7 +2430,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2495,7 +2477,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2542,7 +2524,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2586,7 +2568,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2633,7 +2615,7 @@
         <v>13.4</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2680,7 +2662,7 @@
         <v>20.6</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2727,7 +2709,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2774,7 +2756,7 @@
         <v>14.6</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2821,7 +2803,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2868,7 +2850,7 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2915,7 +2897,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2962,7 +2944,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3009,7 +2991,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3056,7 +3038,7 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3103,7 +3085,7 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3150,7 +3132,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3197,7 +3179,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3244,7 +3226,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3291,7 +3273,7 @@
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3338,7 +3320,7 @@
         <v>17.8</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3385,7 +3367,7 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3432,7 +3414,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3476,7 +3458,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3523,7 +3505,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3567,7 +3549,7 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3614,7 +3596,7 @@
         <v>14.6</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3661,7 +3643,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3708,7 +3690,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3755,10 +3737,8 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A74" s="1" t="s">
-        <v>20</v>
-      </c>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -3767,10 +3747,8 @@
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A75" s="1" t="s">
-        <v>15</v>
-      </c>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -3779,10 +3757,8 @@
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A76" s="1" t="s">
-        <v>16</v>
-      </c>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -3791,10 +3767,8 @@
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A77" s="1" t="s">
-        <v>17</v>
-      </c>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -3803,10 +3777,8 @@
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A78" s="1" t="s">
-        <v>18</v>
-      </c>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -3815,10 +3787,8 @@
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A79" s="1" t="s">
-        <v>19</v>
-      </c>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -3827,7 +3797,7 @@
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>

</xml_diff>

<commit_message>
Replaced empty cells with 0s
</commit_message>
<xml_diff>
--- a/jss13_ht20.xlsx
+++ b/jss13_ht20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\redho\Documents\gits\labAssignmentsForStatisticalMethods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD18A50-15AA-419B-9C08-02C1B02FA1BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652ED934-874A-46AE-A280-C28879BE8E47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="38700" windowHeight="15435" xr2:uid="{039FF9D7-ACF4-48DA-B635-5B4DE3137A46}"/>
+    <workbookView xWindow="9165" yWindow="14085" windowWidth="38700" windowHeight="15435" xr2:uid="{039FF9D7-ACF4-48DA-B635-5B4DE3137A46}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -425,7 +425,7 @@
   <dimension ref="A1:O80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E77" sqref="E77"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,6 +496,9 @@
       <c r="F2">
         <v>4</v>
       </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
       <c r="H2">
         <v>10</v>
       </c>
@@ -508,6 +511,9 @@
       <c r="K2">
         <v>3</v>
       </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
       <c r="M2">
         <v>1</v>
       </c>
@@ -536,6 +542,9 @@
       </c>
       <c r="F3">
         <v>2</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
       </c>
       <c r="H3">
         <v>7</v>
@@ -766,6 +775,9 @@
       <c r="E8">
         <v>2</v>
       </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
       <c r="G8">
         <v>11</v>
       </c>
@@ -1025,6 +1037,9 @@
       <c r="N13">
         <v>4</v>
       </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1445,6 +1460,9 @@
       <c r="N22">
         <v>6</v>
       </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -1909,6 +1927,9 @@
       <c r="M32">
         <v>2</v>
       </c>
+      <c r="N32">
+        <v>99</v>
+      </c>
       <c r="O32">
         <v>14.4</v>
       </c>
@@ -2534,6 +2555,9 @@
       <c r="C46">
         <v>1</v>
       </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
       <c r="E46">
         <v>10</v>
       </c>
@@ -3427,6 +3451,9 @@
       <c r="D65">
         <v>46</v>
       </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
       <c r="F65">
         <v>1</v>
       </c>
@@ -3520,6 +3547,9 @@
       </c>
       <c r="E67">
         <v>8</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
       </c>
       <c r="G67">
         <v>10</v>

</xml_diff>